<commit_message>
Add manufacturers to parts list
</commit_message>
<xml_diff>
--- a/Lab2.X/F14 PCB parts list.xlsx
+++ b/Lab2.X/F14 PCB parts list.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\MSU\Embed Sys\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thesh\Documents\MSU\terms\spring_2020\embedded\lab\files\Lab2\Lab2.X\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C34CCA21-B0B6-44C3-9584-D0F9E3B9BA24}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C8374A2-4E42-42E3-BA17-9CCFF7356DFE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1068" yWindow="-108" windowWidth="22080" windowHeight="13176" xr2:uid="{F7341976-5CE6-4590-9369-0D7B06F7A062}"/>
+    <workbookView xWindow="5700" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{F7341976-5CE6-4590-9369-0D7B06F7A062}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="87">
   <si>
     <t>Part Name</t>
   </si>
@@ -262,6 +262,36 @@
   </si>
   <si>
     <t>na</t>
+  </si>
+  <si>
+    <t>Kingbright</t>
+  </si>
+  <si>
+    <t>TE Connectivity</t>
+  </si>
+  <si>
+    <t>FTDI (?)</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Vishay</t>
+  </si>
+  <si>
+    <t>ALPS</t>
+  </si>
+  <si>
+    <t>Alpha (Taiwan)</t>
+  </si>
+  <si>
+    <t>Panasonic</t>
+  </si>
+  <si>
+    <t>KEMET</t>
+  </si>
+  <si>
+    <t>Murata</t>
   </si>
 </sst>
 </file>
@@ -738,22 +768,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5B82B82-34EE-4B94-980A-398253693AB3}">
   <dimension ref="A3:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.109375" customWidth="1"/>
-    <col min="2" max="2" width="19.109375" customWidth="1"/>
-    <col min="3" max="3" width="20.33203125" customWidth="1"/>
-    <col min="4" max="4" width="6.5546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="29.44140625" customWidth="1"/>
-    <col min="6" max="6" width="5.109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="39.44140625" customWidth="1"/>
+    <col min="1" max="1" width="17.140625" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" customWidth="1"/>
+    <col min="4" max="4" width="6.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="29.42578125" customWidth="1"/>
+    <col min="6" max="6" width="5.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="39.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -776,7 +806,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -793,7 +823,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>86</v>
+      </c>
       <c r="B5" t="s">
         <v>10</v>
       </c>
@@ -813,7 +846,10 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>85</v>
+      </c>
       <c r="B6" t="s">
         <v>33</v>
       </c>
@@ -833,7 +869,10 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>81</v>
+      </c>
       <c r="B7" t="s">
         <v>21</v>
       </c>
@@ -853,7 +892,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>30</v>
       </c>
@@ -876,8 +915,10 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="7"/>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>85</v>
+      </c>
       <c r="B9" s="8" t="s">
         <v>34</v>
       </c>
@@ -897,8 +938,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="7"/>
+    <row r="10" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>84</v>
+      </c>
       <c r="B10" s="8" t="s">
         <v>18</v>
       </c>
@@ -918,8 +961,10 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="7"/>
+    <row r="11" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>81</v>
+      </c>
       <c r="B11" s="8" t="s">
         <v>39</v>
       </c>
@@ -937,8 +982,10 @@
       </c>
       <c r="G11" s="10"/>
     </row>
-    <row r="12" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="7"/>
+    <row r="12" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>77</v>
+      </c>
       <c r="B12" s="8" t="s">
         <v>40</v>
       </c>
@@ -956,8 +1003,10 @@
       </c>
       <c r="G12" s="10"/>
     </row>
-    <row r="13" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="7"/>
+    <row r="13" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>80</v>
+      </c>
       <c r="B13" s="8" t="s">
         <v>43</v>
       </c>
@@ -977,8 +1026,10 @@
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="11"/>
+    <row r="14" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="s">
+        <v>78</v>
+      </c>
       <c r="B14" s="12" t="s">
         <v>46</v>
       </c>
@@ -996,7 +1047,10 @@
       </c>
       <c r="G14" s="14"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>78</v>
+      </c>
       <c r="B15" t="s">
         <v>27</v>
       </c>
@@ -1013,7 +1067,10 @@
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>83</v>
+      </c>
       <c r="B16" t="s">
         <v>48</v>
       </c>
@@ -1030,7 +1087,10 @@
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>82</v>
+      </c>
       <c r="B17" t="s">
         <v>52</v>
       </c>
@@ -1047,7 +1107,10 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>77</v>
+      </c>
       <c r="B18" t="s">
         <v>35</v>
       </c>
@@ -1064,7 +1127,10 @@
         <v>55</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>81</v>
+      </c>
       <c r="B19" t="s">
         <v>38</v>
       </c>
@@ -1084,7 +1150,10 @@
         <v>75</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>81</v>
+      </c>
       <c r="B20" t="s">
         <v>57</v>
       </c>
@@ -1104,7 +1173,10 @@
         <v>59</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>78</v>
+      </c>
       <c r="B21" t="s">
         <v>60</v>
       </c>
@@ -1121,7 +1193,10 @@
         <v>55</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>78</v>
+      </c>
       <c r="B22" t="s">
         <v>63</v>
       </c>
@@ -1138,7 +1213,10 @@
         <v>55</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>79</v>
+      </c>
       <c r="B23" t="s">
         <v>66</v>
       </c>
@@ -1155,7 +1233,10 @@
         <v>68</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
+        <v>80</v>
+      </c>
       <c r="B24" t="s">
         <v>69</v>
       </c>
@@ -1172,7 +1253,10 @@
         <v>68</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
+        <v>80</v>
+      </c>
       <c r="B25" t="s">
         <v>69</v>
       </c>

</xml_diff>